<commit_message>
Update reporting for 29th Jan
</commit_message>
<xml_diff>
--- a/scripts/all-ci-times.xlsx
+++ b/scripts/all-ci-times.xlsx
@@ -5,16 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rikki\src\roslyn\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rikki\src\roslyn2\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94E7462-404C-4198-B9AE-8E3E5B7D614B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56A75FB-40BE-4A8A-9262-C9B73AEE8D03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="2730" windowWidth="26145" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7770" yWindow="5685" windowWidth="26145" windowHeight="15150" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="successful runs (15 dec 2020)" sheetId="7" r:id="rId1"/>
     <sheet name="successful runs (21 jan 2021)" sheetId="8" r:id="rId2"/>
+    <sheet name="master runs (21 jan 2021)" sheetId="9" r:id="rId3"/>
+    <sheet name="master runs (29 jan 2021)" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
   <si>
     <t>runId</t>
   </si>
@@ -2507,6 +2509,1859 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>roslyn-ci</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> master run times (14th-21st Jan 2021)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'master runs (21 jan 2021)'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prereqFinish</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'master runs (21 jan 2021)'!$C$2:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0_Run_Created</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1_Build_Windows_Debug</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2_Test_Windows_CoreClr_Debug</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2_Test_Windows_Desktop_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2_Test_Windows_Desktop_Debug_64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2_Test_Windows_Desktop_Spanish_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3_Build_Windows_Release</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4_Test_Windows_CoreClr_Release</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4_Test_Windows_Desktop_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4_Test_Windows_Desktop_Release_64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4_Test_Windows_Desktop_Spanish_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5_Build_Unix_Debug</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6_Test_Linux_Debug</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_Test_macOS_Debug</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_Correctness_Build</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7_Correctness_Determinism</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7_Correctness_SourceBuild</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'master runs (21 jan 2021)'!$E$2:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="mm:ss.0">
+                  <c:v>1.1747615740740742E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="mm:ss.0">
+                  <c:v>1.1747615740740742E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="mm:ss.0">
+                  <c:v>1.1747615740740742E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="mm:ss.0">
+                  <c:v>1.4771747685185186E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="mm:ss.0">
+                  <c:v>1.4771747685185186E-2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="mm:ss.0">
+                  <c:v>1.4771747685185186E-2</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="mm:ss.0">
+                  <c:v>1.4771747685185186E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="mm:ss.0">
+                  <c:v>7.9142824074074063E-3</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="mm:ss.0">
+                  <c:v>7.9142824074074063E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6234-4547-BBC7-D48C51463ED6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'master runs (21 jan 2021)'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>startDelay</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-6234-4547-BBC7-D48C51463ED6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'master runs (21 jan 2021)'!$C$2:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0_Run_Created</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1_Build_Windows_Debug</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2_Test_Windows_CoreClr_Debug</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2_Test_Windows_Desktop_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2_Test_Windows_Desktop_Debug_64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2_Test_Windows_Desktop_Spanish_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3_Build_Windows_Release</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4_Test_Windows_CoreClr_Release</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4_Test_Windows_Desktop_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4_Test_Windows_Desktop_Release_64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4_Test_Windows_Desktop_Spanish_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5_Build_Unix_Debug</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6_Test_Linux_Debug</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_Test_macOS_Debug</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_Correctness_Build</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7_Correctness_Determinism</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7_Correctness_SourceBuild</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'master runs (21 jan 2021)'!$F$2:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8799189814814816E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8662152777777779E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7927893518518523E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2654166666666665E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1700694444444445E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.147418981481482E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.3906828703703703E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.3746180555555561E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.3360648148148152E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0033564814814819E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.2386574074074081E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.335648148148148E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.189409722222222E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.2796296296296298E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.8121412037037031E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-6234-4547-BBC7-D48C51463ED6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'master runs (21 jan 2021)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'master runs (21 jan 2021)'!$C$2:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0_Run_Created</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1_Build_Windows_Debug</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2_Test_Windows_CoreClr_Debug</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2_Test_Windows_Desktop_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2_Test_Windows_Desktop_Debug_64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2_Test_Windows_Desktop_Spanish_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3_Build_Windows_Release</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4_Test_Windows_CoreClr_Release</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4_Test_Windows_Desktop_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4_Test_Windows_Desktop_Release_64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4_Test_Windows_Desktop_Spanish_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5_Build_Unix_Debug</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6_Test_Linux_Debug</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_Test_macOS_Debug</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_Correctness_Build</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7_Correctness_Determinism</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7_Correctness_SourceBuild</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'master runs (21 jan 2021)'!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8676967592592592E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5132523148148147E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7224675925925926E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7017037037037037E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3601689814814813E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.6857407407407413E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2497870370370373E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2316828703703707E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2556909722222223E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.4139351851851857E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.8128935185185176E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.9449884259259257E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3202789351851853E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.0218113425925926E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.037310185185185E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6234-4547-BBC7-D48C51463ED6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="218924031"/>
+        <c:axId val="218924447"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="218924031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="218924447"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="218924447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="h:mm:ss" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="218924031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>roslyn-ci</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> master run times (22th-29th Jan 2021)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'master runs (29 jan 2021)'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prereqFinish</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'master runs (29 jan 2021)'!$C$2:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0_Run_Created</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1_Build_Windows_Debug</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2_Test_Windows_CoreClr_Debug</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2_Test_Windows_Desktop_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2_Test_Windows_Desktop_Debug_64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2_Test_Windows_Desktop_Spanish_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3_Build_Windows_Release</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4_Test_Windows_CoreClr_Release</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4_Test_Windows_Desktop_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4_Test_Windows_Desktop_Release_64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4_Test_Windows_Desktop_Spanish_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5_Build_Unix_Debug</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6_Test_Linux_Debug</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_Test_macOS_Debug</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_Correctness_Build</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7_Correctness_Determinism</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7_Correctness_SourceBuild</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'master runs (29 jan 2021)'!$E$2:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="mm:ss.0">
+                  <c:v>1.4258136574074076E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="mm:ss.0">
+                  <c:v>1.4258136574074076E-2</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="mm:ss.0">
+                  <c:v>1.4258136574074076E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="mm:ss.0">
+                  <c:v>1.32628125E-2</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="mm:ss.0">
+                  <c:v>1.32628125E-2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="mm:ss.0">
+                  <c:v>1.32628125E-2</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="mm:ss.0">
+                  <c:v>1.32628125E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="mm:ss.0">
+                  <c:v>6.4817013888888893E-3</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="mm:ss.0">
+                  <c:v>6.4817013888888893E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BDDC-4658-A875-FECA4608293C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'master runs (29 jan 2021)'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>startDelay</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-BDDC-4658-A875-FECA4608293C}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'master runs (29 jan 2021)'!$C$2:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0_Run_Created</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1_Build_Windows_Debug</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2_Test_Windows_CoreClr_Debug</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2_Test_Windows_Desktop_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2_Test_Windows_Desktop_Debug_64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2_Test_Windows_Desktop_Spanish_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3_Build_Windows_Release</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4_Test_Windows_CoreClr_Release</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4_Test_Windows_Desktop_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4_Test_Windows_Desktop_Release_64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4_Test_Windows_Desktop_Spanish_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5_Build_Unix_Debug</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6_Test_Linux_Debug</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_Test_macOS_Debug</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_Correctness_Build</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7_Correctness_Determinism</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7_Correctness_SourceBuild</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'master runs (29 jan 2021)'!$F$2:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4762962962962959E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4230671296296298E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7046759259259261E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5125115740740741E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4608796296296295E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2667592592592594E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3923263888888889E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1272453703703703E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5293171296296296E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0380787037037039E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5241550925925928E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.2391203703703705E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.9034259259259266E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.8355208333333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.3864583333333326E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BDDC-4658-A875-FECA4608293C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'master runs (29 jan 2021)'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'master runs (29 jan 2021)'!$C$2:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0_Run_Created</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1_Build_Windows_Debug</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2_Test_Windows_CoreClr_Debug</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2_Test_Windows_Desktop_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2_Test_Windows_Desktop_Debug_64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2_Test_Windows_Desktop_Spanish_Debug_32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3_Build_Windows_Release</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4_Test_Windows_CoreClr_Release</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4_Test_Windows_Desktop_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4_Test_Windows_Desktop_Release_64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4_Test_Windows_Desktop_Spanish_Release_32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5_Build_Unix_Debug</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6_Test_Linux_Debug</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6_Test_macOS_Debug</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7_Correctness_Build</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7_Correctness_Determinism</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7_Correctness_SourceBuild</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'master runs (29 jan 2021)'!$G$2:$G$18</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.0</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7818287037037032E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5953171296296295E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0158796296296296E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0193912037037038E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="h:mm:ss">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2716724537037037E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7213078703703703E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.011390046296296E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9320208333333335E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1608229166666663E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.9778819444444445E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0162407407407406E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7670949074074074E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.3108553240740742E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9575300925925927E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0077962962962964E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-BDDC-4658-A875-FECA4608293C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="218924031"/>
+        <c:axId val="218924447"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="218924031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="218924447"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="218924447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="h:mm:ss" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="218924031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2587,6 +4442,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -3093,6 +5028,1016 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3661,6 +6606,92 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4C7CF86-BB4F-484C-A98A-6B62B06A25DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0262FC77-2E95-4C36-BC3B-50C280F19824}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB7903CD-054B-4C50-BB49-AF2CAE285132}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3983,7 +7014,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -4857,4 +7888,894 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF37E670-0BC9-4452-8B33-6BDFB2430D3B}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.8799189814814816E-3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.8799189814814816E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8.8676967592592592E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.5613831018518516E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.1747615740740742E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.8662152777777779E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>9.5132523148148147E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.5540405092592592E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.1747615740740742E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.7927893518518523E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.7224675925925926E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.6013032407407406E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.1747615740740742E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.2654166666666665E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.7017037037037037E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.1700694444444445E-3</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.1700694444444445E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.3601689814814813E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.8919166666666667E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.4771747685185186E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>4.147418981481482E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>9.6857407407407413E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.9162442129629628E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.4771747685185186E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>4.3906828703703703E-3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.2497870370370373E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.9146365740740742E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.4771747685185186E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4.3746180555555561E-3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.2316828703703707E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.2107812500000001E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.4771747685185186E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>7.3360648148148152E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.2556909722222223E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.0033564814814819E-4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5.0033564814814819E-4</v>
+      </c>
+      <c r="G13" s="2">
+        <v>7.4139351851851857E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.5152939814814815E-2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>7.9142824074074063E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>7.2386574074074081E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>6.8128935185185176E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2">
+        <v>8.2478356481481482E-3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>7.9142824074074063E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3.335648148148148E-4</v>
+      </c>
+      <c r="G15" s="2">
+        <v>8.9449884259259257E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5.189409722222222E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5.189409722222222E-3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.3202789351851853E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5.2796296296296298E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5.2796296296296298E-3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2.0218113425925926E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2">
+        <v>6.8121412037037031E-3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6.8121412037037031E-3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.037310185185185E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC2449C-46F5-4EAA-93EF-E7732A60F915}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="43.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.4762962962962959E-3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5.4762962962962959E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8.7818287037037032E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.568119212962963E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.4258136574074076E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.4230671296296298E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.5953171296296295E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.5962812500000003E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.4258136574074076E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.7046759259259261E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.0158796296296296E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.5770648148148148E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.4258136574074076E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.5125115740740741E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2.0193912037037038E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.4608796296296295E-4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5.4608796296296295E-4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.2716724537037037E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.4529571759259258E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.32628125E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.2667592592592594E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.7213078703703703E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.4655138888888889E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.32628125E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.3923263888888889E-3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2.011390046296296E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.4390057870370371E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.32628125E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.1272453703703703E-3</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.9320208333333335E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.5792129629629628E-2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.32628125E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2.5293171296296296E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2.1608229166666663E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.0380787037037039E-4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5.0380787037037039E-4</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5.9778819444444445E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8.0058449074074077E-3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>6.4817013888888893E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.5241550925925928E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.0162407407407406E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6.8056018518518509E-3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>6.4817013888888893E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3.2391203703703705E-4</v>
+      </c>
+      <c r="G15" s="2">
+        <v>4.7670949074074074E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2">
+        <v>7.9034259259259266E-3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>7.9034259259259266E-3</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.3108553240740742E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2">
+        <v>7.8355208333333332E-3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>7.8355208333333332E-3</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.9575300925925927E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7.3864583333333326E-3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>7.3864583333333326E-3</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1.0077962962962964E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>